<commit_message>
shippingBox and palette cases clean
</commit_message>
<xml_diff>
--- a/Cases/Benchmarking/courantNumberStudy/courant_number.xlsx
+++ b/Cases/Benchmarking/courantNumberStudy/courant_number.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\sbreen\TransportTemperatureModel\Cases\Benchmarking\courant_number\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\sbreen\TransportTemperatureModel\Cases\Benchmarking\courantNumberStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C71B13-1670-4A2B-854D-A17514F6C961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D4B39D-A07A-4526-885F-81846C47B763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22230" yWindow="3570" windowWidth="21480" windowHeight="13935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="990" windowWidth="21480" windowHeight="13935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -354,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:F8"/>
+  <dimension ref="C2:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,6 +433,39 @@
         <v>64</v>
       </c>
     </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>64</v>
+      </c>
+      <c r="E9">
+        <v>36.11</v>
+      </c>
+      <c r="F9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>128</v>
+      </c>
+      <c r="E10">
+        <v>19.260000000000002</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>256</v>
+      </c>
+      <c r="E11">
+        <v>10.56</v>
+      </c>
+      <c r="F11">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>